<commit_message>
final commit in shaa Allah
</commit_message>
<xml_diff>
--- a/Charts & Graphs/ApproximationRatio.xlsx
+++ b/Charts & Graphs/ApproximationRatio.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mylox\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works 2015\mars-workspace\Offline01\Charts &amp; Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -229,37 +229,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>26.0655</c:v>
+                  <c:v>23.722300000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>200.6523</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267.03829999999999</c:v>
+                  <c:v>157.27529999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>519.27880000000005</c:v>
+                  <c:v>233.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>577.74149999999997</c:v>
+                  <c:v>371.09640000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>571.92629999999997</c:v>
+                  <c:v>376.25450000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>581.70079999999996</c:v>
+                  <c:v>387.69389999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>586.14880000000005</c:v>
+                  <c:v>394.65120000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>212.42320000000001</c:v>
+                  <c:v>113.40179999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>286.2362</c:v>
+                  <c:v>140.398</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>238.15049999999999</c:v>
+                  <c:v>141.2585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -330,37 +330,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>26.0655</c:v>
+                  <c:v>26.508500000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>225.26849999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267.03829999999999</c:v>
+                  <c:v>170.8321</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>640.70280000000002</c:v>
+                  <c:v>267.31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>643.99530000000004</c:v>
+                  <c:v>444.2998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>695.81949999999995</c:v>
+                  <c:v>418.84820000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>702.7912</c:v>
+                  <c:v>405.78190000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>650.67819999999995</c:v>
+                  <c:v>466.03190000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>277.17309999999998</c:v>
+                  <c:v>129.03370000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>325.298</c:v>
+                  <c:v>155.43559999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>274.31740000000002</c:v>
+                  <c:v>159.94800000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -376,11 +376,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1379321424"/>
-        <c:axId val="1379327408"/>
+        <c:axId val="-708821968"/>
+        <c:axId val="-708821424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1379321424"/>
+        <c:axId val="-708821968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,7 +479,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1379327408"/>
+        <c:crossAx val="-708821424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -487,7 +487,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1379327408"/>
+        <c:axId val="-708821424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1379321424"/>
+        <c:crossAx val="-708821968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -849,37 +849,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>26.0655</c:v>
+                  <c:v>23.722300000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>200.6523</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267.03829999999999</c:v>
+                  <c:v>157.27529999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>519.27880000000005</c:v>
+                  <c:v>233.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>577.74149999999997</c:v>
+                  <c:v>371.09640000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>571.92629999999997</c:v>
+                  <c:v>376.25450000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>581.70079999999996</c:v>
+                  <c:v>387.69389999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>586.14880000000005</c:v>
+                  <c:v>394.65120000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>212.42320000000001</c:v>
+                  <c:v>113.40179999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>286.2362</c:v>
+                  <c:v>140.398</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>238.15049999999999</c:v>
+                  <c:v>141.2585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -965,37 +965,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>26.0655</c:v>
+                  <c:v>26.508500000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>225.26849999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267.03829999999999</c:v>
+                  <c:v>170.8321</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>640.70280000000002</c:v>
+                  <c:v>267.31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>643.99530000000004</c:v>
+                  <c:v>444.2998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>695.81949999999995</c:v>
+                  <c:v>418.84820000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>702.7912</c:v>
+                  <c:v>405.78190000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>650.67819999999995</c:v>
+                  <c:v>466.03190000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>277.17309999999998</c:v>
+                  <c:v>129.03370000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>325.298</c:v>
+                  <c:v>155.43559999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>274.31740000000002</c:v>
+                  <c:v>159.94800000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1010,11 +1010,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1379377568"/>
-        <c:axId val="1379381376"/>
+        <c:axId val="-891823376"/>
+        <c:axId val="-891828272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1379377568"/>
+        <c:axId val="-891823376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1127,12 +1127,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1379381376"/>
+        <c:crossAx val="-891828272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1379381376"/>
+        <c:axId val="-891828272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,7 +1245,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1379377568"/>
+        <c:crossAx val="-891823376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2756,7 +2756,7 @@
   <dimension ref="B4:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+      <selection activeCell="C4" sqref="C4:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,10 +2769,10 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>26.0655</v>
+        <v>23.722300000000001</v>
       </c>
       <c r="D4">
-        <v>26.0655</v>
+        <v>26.508500000000002</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -2791,10 +2791,10 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>267.03829999999999</v>
+        <v>157.27529999999999</v>
       </c>
       <c r="D6">
-        <v>267.03829999999999</v>
+        <v>170.8321</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2802,10 +2802,10 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>519.27880000000005</v>
+        <v>233.66</v>
       </c>
       <c r="D7">
-        <v>640.70280000000002</v>
+        <v>267.31</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -2813,10 +2813,10 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>577.74149999999997</v>
+        <v>371.09640000000002</v>
       </c>
       <c r="D8">
-        <v>643.99530000000004</v>
+        <v>444.2998</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -2824,10 +2824,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>571.92629999999997</v>
+        <v>376.25450000000001</v>
       </c>
       <c r="D9">
-        <v>695.81949999999995</v>
+        <v>418.84820000000002</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -2835,10 +2835,10 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>581.70079999999996</v>
+        <v>387.69389999999999</v>
       </c>
       <c r="D10">
-        <v>702.7912</v>
+        <v>405.78190000000001</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -2846,10 +2846,10 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>586.14880000000005</v>
+        <v>394.65120000000002</v>
       </c>
       <c r="D11">
-        <v>650.67819999999995</v>
+        <v>466.03190000000001</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -2857,10 +2857,10 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>212.42320000000001</v>
+        <v>113.40179999999999</v>
       </c>
       <c r="D12">
-        <v>277.17309999999998</v>
+        <v>129.03370000000001</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -2868,10 +2868,10 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>286.2362</v>
+        <v>140.398</v>
       </c>
       <c r="D13">
-        <v>325.298</v>
+        <v>155.43559999999999</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -2879,10 +2879,10 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>238.15049999999999</v>
+        <v>141.2585</v>
       </c>
       <c r="D14">
-        <v>274.31740000000002</v>
+        <v>159.94800000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>